<commit_message>
updated custom app bar button
</commit_message>
<xml_diff>
--- a/selenium_web_scrapper_python/data_product.xlsx
+++ b/selenium_web_scrapper_python/data_product.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -40,6 +40,12 @@
     <t>0741b8ff-7918-4b20-b049-6b5660e40218</t>
   </si>
   <si>
+    <t>f8c6fc0f-c983-4edd-8fa7-72454eedcb2c</t>
+  </si>
+  <si>
+    <t>76ab1cfe-bffc-46e5-b6e1-9f3ecdc24b52</t>
+  </si>
+  <si>
     <t>CORSAIR VENGEANCE® LPX 8GB DDR4 DRAM 3200MHz CMK8GX4M1E3200C16</t>
   </si>
   <si>
@@ -49,6 +55,12 @@
     <t>RAM IMPERION RGB DDR4 16GB (2X8GB) 2666MHz KIT RAM PC RGB GAMING RESMI - 8GB (1X8GB)</t>
   </si>
   <si>
+    <t>RAM KINGSTON HYPERX FURY DDR4 8GB 2666MHz 21300 GAMING RAM PC DDR4 8GB</t>
+  </si>
+  <si>
+    <t>RAM DDR4 V-GeN RESCUE 8GB PC19200/2400Mhz Long Dimm (Memory PC VGEN)</t>
+  </si>
+  <si>
     <t>Tokopedia</t>
   </si>
   <si>
@@ -59,6 +71,12 @@
   </si>
   <si>
     <t>https://www.tokopedia.com/rajaramnusantara/ram-imperion-rgb-ddr4-16gb-2x8gb-2666mhz-kit-ram-pc-rgb-gaming-resmi-8gb-1x8gb?src=topads</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/rajaramnusantara/ram-kingston-hyperx-fury-ddr4-8gb-2666mhz-21300-gaming-ram-pc-ddr4-8gb?src=topads</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/intact-official/ram-ddr4-v-gen-rescue-8gb-pc19200-2400mhz-long-dimm-memory-pc-vgen?extParam=ivf%3Dfalse%26src%3Dsearch</t>
   </si>
 </sst>
 </file>
@@ -429,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,16 +478,16 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F2">
-        <v>659000</v>
+        <v>629000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -480,13 +498,13 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>664050</v>
@@ -500,16 +518,56 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>549000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
+        <v>390000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
-        <v>589000</v>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>458000</v>
       </c>
     </row>
   </sheetData>
@@ -517,6 +575,8 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>